<commit_message>
fixed row count issue
</commit_message>
<xml_diff>
--- a/src/main/java/com/junithybrid/xlsx/Check_Items.xlsx
+++ b/src/main/java/com/junithybrid/xlsx/Check_Items.xlsx
@@ -35,160 +35,160 @@
     <t>Login to the application</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>CheckItems</t>
+  </si>
+  <si>
+    <t>Check the items in various categories</t>
+  </si>
+  <si>
+    <t>AddItemsToCard</t>
+  </si>
+  <si>
+    <t>Add the items into the cart</t>
+  </si>
+  <si>
+    <t>testId</t>
+  </si>
+  <si>
+    <t>Test description</t>
+  </si>
+  <si>
+    <t>TSTEPS_ID</t>
+  </si>
+  <si>
+    <t>TSTEPS_Description</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Proceed_on_Fail</t>
+  </si>
+  <si>
+    <t>TS01</t>
+  </si>
+  <si>
+    <t>Open browser</t>
+  </si>
+  <si>
+    <t>openBrowser</t>
+  </si>
+  <si>
+    <t>TS02</t>
+  </si>
+  <si>
+    <t>Navigate to site</t>
+  </si>
+  <si>
+    <t>navigate</t>
+  </si>
+  <si>
+    <t>TS03</t>
+  </si>
+  <si>
+    <t>Check title</t>
+  </si>
+  <si>
+    <t>verifyTitle</t>
+  </si>
+  <si>
+    <t>TS04</t>
+  </si>
+  <si>
+    <t>Check the login like</t>
+  </si>
+  <si>
+    <t>clickLink</t>
+  </si>
+  <si>
+    <t>TS05</t>
+  </si>
+  <si>
+    <t>Enter username</t>
+  </si>
+  <si>
+    <t>writeInInput</t>
+  </si>
+  <si>
+    <t>TS06</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>TS07</t>
+  </si>
+  <si>
+    <t>Click submit button</t>
+  </si>
+  <si>
+    <t>clickButton</t>
+  </si>
+  <si>
+    <t>TS08</t>
+  </si>
+  <si>
+    <t>Check the logout link</t>
+  </si>
+  <si>
+    <t>verifyLinkText</t>
+  </si>
+  <si>
+    <t>Click on category</t>
+  </si>
+  <si>
+    <t>checkLink</t>
+  </si>
+  <si>
+    <t>Verify item</t>
+  </si>
+  <si>
+    <t>Verify item price</t>
+  </si>
+  <si>
+    <t>verifyText</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>c1v1</t>
+  </si>
+  <si>
+    <t>c2v1</t>
+  </si>
+  <si>
+    <t>c1v2</t>
+  </si>
+  <si>
+    <t>c2v2</t>
+  </si>
+  <si>
+    <t>c1v3</t>
+  </si>
+  <si>
+    <t>c2v3</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>CheckItems</t>
-  </si>
-  <si>
-    <t>Check the items in various categories</t>
-  </si>
-  <si>
-    <t>AddItemsToCard</t>
-  </si>
-  <si>
-    <t>Add the items into the cart</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>testId</t>
-  </si>
-  <si>
-    <t>Test description</t>
-  </si>
-  <si>
-    <t>TSTEPS_ID</t>
-  </si>
-  <si>
-    <t>TSTEPS_Description</t>
-  </si>
-  <si>
-    <t>Keyword</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Proceed_on_Fail</t>
-  </si>
-  <si>
-    <t>TS01</t>
-  </si>
-  <si>
-    <t>Open browser</t>
-  </si>
-  <si>
-    <t>openBrowser</t>
-  </si>
-  <si>
-    <t>TS02</t>
-  </si>
-  <si>
-    <t>Navigate to site</t>
-  </si>
-  <si>
-    <t>navigate</t>
-  </si>
-  <si>
-    <t>TS03</t>
-  </si>
-  <si>
-    <t>Check title</t>
-  </si>
-  <si>
-    <t>verifyTitle</t>
-  </si>
-  <si>
-    <t>TS04</t>
-  </si>
-  <si>
-    <t>Check the login like</t>
-  </si>
-  <si>
-    <t>clickLink</t>
-  </si>
-  <si>
-    <t>TS05</t>
-  </si>
-  <si>
-    <t>Enter username</t>
-  </si>
-  <si>
-    <t>writeInInput</t>
-  </si>
-  <si>
-    <t>TS06</t>
-  </si>
-  <si>
-    <t>Enter password</t>
-  </si>
-  <si>
-    <t>TS07</t>
-  </si>
-  <si>
-    <t>Click submit button</t>
-  </si>
-  <si>
-    <t>clickButton</t>
-  </si>
-  <si>
-    <t>TS08</t>
-  </si>
-  <si>
-    <t>Check the logout link</t>
-  </si>
-  <si>
-    <t>verifyLinkText</t>
-  </si>
-  <si>
-    <t>Click on category</t>
-  </si>
-  <si>
-    <t>checkLink</t>
-  </si>
-  <si>
-    <t>Verify item</t>
-  </si>
-  <si>
-    <t>Verify item price</t>
-  </si>
-  <si>
-    <t>verifyText</t>
-  </si>
-  <si>
-    <t>Col1</t>
-  </si>
-  <si>
-    <t>Col2</t>
-  </si>
-  <si>
-    <t>RunMode</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>c1v1</t>
-  </si>
-  <si>
-    <t>c2v1</t>
-  </si>
-  <si>
-    <t>c1v2</t>
-  </si>
-  <si>
-    <t>c2v2</t>
-  </si>
-  <si>
-    <t>c1v3</t>
-  </si>
-  <si>
-    <t>c2v3</t>
   </si>
   <si>
     <t>c1v4</t>
@@ -458,7 +458,7 @@
   <dimension ref="A1:C65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -509,20 +509,30 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -544,7 +554,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -563,22 +573,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,13 +596,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -603,13 +613,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -620,13 +630,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -637,13 +647,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -654,13 +664,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -671,13 +681,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -688,13 +698,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -705,13 +715,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -722,13 +732,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -739,13 +749,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -756,13 +766,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -773,13 +783,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -790,13 +800,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -807,13 +817,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -824,13 +834,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -841,13 +851,13 @@
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -858,13 +868,13 @@
         <v>8</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -875,13 +885,13 @@
         <v>8</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -892,13 +902,13 @@
         <v>8</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -909,13 +919,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -926,13 +936,13 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -957,7 +967,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -969,49 +979,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,7 +1032,7 @@
         <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1054,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1071,10 +1081,10 @@
         <v>63</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,7 +1101,7 @@
         <v>66</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,7 +1118,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,7 +1135,7 @@
         <v>72</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,7 +1152,7 @@
         <v>75</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Keywords.java and DriverScript.java
</commit_message>
<xml_diff>
--- a/src/main/java/com/junithybrid/xlsx/Check_Items.xlsx
+++ b/src/main/java/com/junithybrid/xlsx/Check_Items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,6 +44,9 @@
     <t>Check the items in various categories</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>AddItemsToCard</t>
   </si>
   <si>
@@ -186,9 +189,6 @@
   </si>
   <si>
     <t>c2v3</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>c1v4</t>
@@ -457,8 +457,8 @@
   </sheetPr>
   <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -498,29 +498,29 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -573,22 +573,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,13 +596,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -613,13 +613,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -630,13 +630,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -647,13 +647,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -664,13 +664,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -681,13 +681,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -698,13 +698,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -715,13 +715,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -732,13 +732,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -749,13 +749,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -766,13 +766,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -783,13 +783,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -800,13 +800,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -817,13 +817,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -834,13 +834,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -851,13 +851,13 @@
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -865,16 +865,16 @@
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -882,16 +882,16 @@
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -899,16 +899,16 @@
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -916,16 +916,16 @@
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -933,16 +933,16 @@
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -967,7 +967,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -979,24 +979,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
@@ -1004,24 +1004,24 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,7 +1032,7 @@
         <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1053,8 +1053,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1081,10 +1081,10 @@
         <v>63</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1118,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,7 +1135,7 @@
         <v>72</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>